<commit_message>
before graded exercise announcement
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="28800" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="13860" yWindow="2280" windowWidth="28240" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> per Criteria</t>
@@ -143,7 +143,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> per Unit</t>
@@ -172,7 +172,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -589,7 +589,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -635,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -658,11 +658,11 @@
       </c>
       <c r="G6" s="4">
         <f>SUM(G4:G5)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
         <f>MIN(C6,G6)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -673,7 +673,7 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -684,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -717,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -729,11 +729,11 @@
       </c>
       <c r="G13" s="4">
         <f>SUM(G8:G12)</f>
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H13" s="4">
         <f>MIN(C13,G13)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -748,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:9">
@@ -770,7 +770,7 @@
         <v>12</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:9">
@@ -781,7 +781,7 @@
         <v>11</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:9">
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:9">
@@ -803,7 +803,7 @@
         <v>15</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -814,7 +814,7 @@
         <v>16</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -826,44 +826,44 @@
       </c>
       <c r="G22" s="4">
         <f>SUM(G15:G21)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H22" s="4">
         <f>MIN(C22,G22)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="D24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
         <v>22</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="D25">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
         <v>21</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9">
       <c r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
         <v>18</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:9">
@@ -874,7 +874,7 @@
         <v>19</v>
       </c>
       <c r="G27">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:9">
@@ -885,7 +885,7 @@
         <v>20</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:9">
@@ -897,11 +897,11 @@
       </c>
       <c r="G29" s="4">
         <f>SUM(G24:G28)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4">
         <f>MIN(C29,G29)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:9">
@@ -913,11 +913,11 @@
       </c>
       <c r="H32">
         <f>SUM(H4:H29)</f>
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <f>MIN(C32,H32)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:9">
@@ -932,7 +932,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="6">
         <f>1 + TOTAL_POINTS/10</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>